<commit_message>
Update on sprint backlog 09-04
</commit_message>
<xml_diff>
--- a/docs/SCRUM/SprintBacklog.xlsx
+++ b/docs/SCRUM/SprintBacklog.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{995B643B-CDF2-4D6B-9152-597D108C4DE2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{76978926-3594-4EEE-AD0A-1A24E2939D38}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{995B643B-CDF2-4D6B-9152-597D108C4DE2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{4385BE4A-F180-4985-9540-C10E5FEA1D0C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>Kategori</t>
   </si>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>Kode aktivitet</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
 </sst>
 </file>
@@ -1021,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="74" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="74" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1355,7 +1349,9 @@
       <c r="H11" s="6">
         <v>0</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -1391,7 +1387,9 @@
       <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1427,7 +1425,9 @@
       <c r="H13" s="4">
         <v>7</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="6">
+        <v>7</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1463,7 +1463,9 @@
       <c r="H14" s="4">
         <v>10</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="6">
+        <v>10</v>
+      </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -1499,7 +1501,9 @@
       <c r="H15" s="6">
         <v>0</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
@@ -1535,7 +1539,9 @@
       <c r="H16" s="6">
         <v>0</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="6"/>
@@ -1571,7 +1577,9 @@
       <c r="H17" s="4">
         <v>0</v>
       </c>
-      <c r="I17" s="6"/>
+      <c r="I17" s="6">
+        <v>0</v>
+      </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -1607,7 +1615,9 @@
       <c r="H18" s="4">
         <v>0</v>
       </c>
-      <c r="I18" s="6"/>
+      <c r="I18" s="6">
+        <v>0</v>
+      </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1643,7 +1653,9 @@
       <c r="H19" s="4">
         <v>0</v>
       </c>
-      <c r="I19" s="6"/>
+      <c r="I19" s="6">
+        <v>0</v>
+      </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="4"/>
@@ -1676,10 +1688,12 @@
       <c r="G20" s="6">
         <v>10</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="4"/>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -1969,7 +1983,9 @@
       <c r="H32" s="4">
         <v>8</v>
       </c>
-      <c r="I32" s="6"/>
+      <c r="I32" s="6">
+        <v>8</v>
+      </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
@@ -2005,7 +2021,9 @@
       <c r="H33" s="4">
         <v>7</v>
       </c>
-      <c r="I33" s="6"/>
+      <c r="I33" s="6">
+        <v>4</v>
+      </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
@@ -2038,10 +2056,12 @@
       <c r="G34" s="6">
         <v>10</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="6"/>
+      <c r="H34" s="6">
+        <v>0</v>
+      </c>
+      <c r="I34" s="6">
+        <v>0</v>
+      </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
       <c r="L34" s="4"/>

</xml_diff>